<commit_message>
Objective changes in fields order
</commit_message>
<xml_diff>
--- a/Tier System/stable version/v02-00/NBO-Microscopy Metadata Tier System_v02-00.xlsx
+++ b/Tier System/stable version/v02-00/NBO-Microscopy Metadata Tier System_v02-00.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Tier System/stable version/v02-00/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955D2521-10E6-1B40-AC89-91871A1C5A89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E27409-C340-CE4E-A929-8EA3353F2AFF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28320" windowHeight="16740" tabRatio="914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,10 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="50">
-  <si>
-    <t>-- required metadata --</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -1334,16 +1331,14 @@
   <sheetData>
     <row r="1" spans="1:13" ht="47" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="64" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="63"/>
       <c r="C1" s="65"/>
       <c r="D1" s="63"/>
       <c r="E1" s="63"/>
       <c r="F1" s="63"/>
-      <c r="G1" s="66" t="s">
-        <v>0</v>
-      </c>
+      <c r="G1" s="66"/>
       <c r="H1" s="66"/>
       <c r="I1" s="66"/>
       <c r="J1" s="63"/>
@@ -1352,113 +1347,113 @@
     </row>
     <row r="2" spans="1:13" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="62" t="s">
+      <c r="E2" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="62" t="s">
+      <c r="G2" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="62" t="s">
+      <c r="K2" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="62" t="s">
-        <v>5</v>
-      </c>
       <c r="L2" s="62" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="343" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="31">
         <v>1</v>
       </c>
       <c r="C3" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="40" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="72" t="s">
         <v>38</v>
-      </c>
-      <c r="K3" s="72" t="s">
-        <v>39</v>
       </c>
       <c r="L3" s="73"/>
       <c r="M3" s="12"/>
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="29">
         <v>2</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="42" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K4" s="74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4" s="75"/>
       <c r="M4" s="6"/>
@@ -1469,27 +1464,27 @@
         <v>3</v>
       </c>
       <c r="C5" s="39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="70"/>
       <c r="I5" s="71"/>
       <c r="J5" s="47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L5" s="76"/>
       <c r="M5" s="7"/>
@@ -1542,7 +1537,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="79" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="79"/>
       <c r="C1" s="79"/>
@@ -1556,100 +1551,100 @@
     </row>
     <row r="2" spans="1:11" s="23" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="58" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="67" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" s="58" t="s">
-        <v>15</v>
       </c>
       <c r="K2" s="22"/>
     </row>
     <row r="3" spans="1:11" s="9" customFormat="1" ht="272" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
       </c>
       <c r="C3" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>20</v>
-      </c>
       <c r="E3" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" s="36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I3" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" ht="359" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="29">
         <v>2</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J4" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -1659,24 +1654,24 @@
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="77"/>
       <c r="I5" s="78"/>
       <c r="J5" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="7"/>
     </row>
@@ -1724,80 +1719,80 @@
   <sheetData>
     <row r="2" spans="1:9" s="23" customFormat="1" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="58" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="58" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="242" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="10" customFormat="1" ht="370" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="29">
         <v>2</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E4" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1806,22 +1801,22 @@
         <v>3</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I5"/>
     </row>

</xml_diff>